<commit_message>
review download upload and excel file to create db
</commit_message>
<xml_diff>
--- a/db/excel/qlns-database-v1.xlsx
+++ b/db/excel/qlns-database-v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DINHNV\MyData\LAPTRINH\NODE4\ionic4.qlns\db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264A88C5-CB77-4489-8890-9CD2CFA22262}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E378A0-F0CF-4729-A015-AA4C8DA7E82B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,8 @@
     <sheet name="form-report-staff" sheetId="36" state="hidden" r:id="rId4"/>
     <sheet name="admin_menu-ver2.0" sheetId="14" state="hidden" r:id="rId5"/>
     <sheet name="organizations" sheetId="9" r:id="rId6"/>
-    <sheet name="job_roles" sheetId="12" r:id="rId7"/>
-    <sheet name="staffs" sheetId="16" r:id="rId8"/>
+    <sheet name="job_roles_sample" sheetId="12" r:id="rId7"/>
+    <sheet name="staffs_sample" sheetId="16" r:id="rId8"/>
     <sheet name="users" sheetId="38" r:id="rId9"/>
     <sheet name="strategy_period" sheetId="39" r:id="rId10"/>
     <sheet name="reports" sheetId="40" r:id="rId11"/>
@@ -29,7 +29,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'admin_menu-ver2.0'!$A$1:$Q$27</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tables!$A$1:$G$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tables!$A$1:$G$39</definedName>
   </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="470">
   <si>
     <t>id</t>
   </si>
@@ -1117,12 +1117,6 @@
     <t>job_list</t>
   </si>
   <si>
-    <t>KT</t>
-  </si>
-  <si>
-    <t>Phòng Kỹ Thuật</t>
-  </si>
-  <si>
     <t>OrganizationsPage</t>
   </si>
   <si>
@@ -1293,24 +1287,12 @@
     <t>Đây là một tổ chức Công ty dùng mô phỏng. Để được gán quyền vào tổ chức, hãy liên hệ với quản trị Tổ chức của bạn.</t>
   </si>
   <si>
-    <t>Phòng Tổng hợp</t>
-  </si>
-  <si>
-    <t>Phòng Kinh doanh</t>
-  </si>
-  <si>
     <t>Tên viết tắt gọn</t>
   </si>
   <si>
     <t>ABC&amp;XYZ</t>
   </si>
   <si>
-    <t>TH</t>
-  </si>
-  <si>
-    <t>KD</t>
-  </si>
-  <si>
     <t>Trưởng phòng</t>
   </si>
   <si>
@@ -1356,9 +1338,6 @@
     <t>Phụ trách phòng</t>
   </si>
   <si>
-    <t>Phụ Trách phòng Tổng hợp</t>
-  </si>
-  <si>
     <t>{"username":"123456789","time":1573185232164,"ip":"10.151.50.36"}</t>
   </si>
   <si>
@@ -1701,7 +1680,10 @@
     <t>[1,2]</t>
   </si>
   <si>
-    <t>Ch? ký c?p nh?p</t>
+    <t>Phụ Trách phòng Kỹ thuật</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -3372,7 +3354,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -3943,6 +3925,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3955,6 +3943,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -3967,12 +3973,6 @@
     <xf numFmtId="0" fontId="35" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -3980,18 +3980,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5391,13 +5379,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G107"/>
+  <dimension ref="A1:G105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomRight" activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5644,7 +5632,9 @@
       <c r="D12" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="E12" s="62"/>
+      <c r="E12" s="62" t="s">
+        <v>469</v>
+      </c>
       <c r="F12" s="40"/>
       <c r="G12" s="16">
         <v>51</v>
@@ -5677,7 +5667,7 @@
         <v>118</v>
       </c>
       <c r="C14" s="177" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="D14" s="177" t="s">
         <v>123</v>
@@ -5757,7 +5747,7 @@
         <v>122</v>
       </c>
       <c r="E18" s="63" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="F18" s="43"/>
       <c r="G18" s="16">
@@ -5937,84 +5927,84 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75">
+    <row r="28" spans="1:7" ht="47.25">
       <c r="A28" s="91" t="s">
         <v>161</v>
       </c>
-      <c r="B28" s="84" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>475</v>
-      </c>
-      <c r="D28" s="212" t="s">
-        <v>123</v>
-      </c>
-      <c r="E28" s="61"/>
-      <c r="F28" s="16"/>
+      <c r="B28" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="F28" s="42"/>
       <c r="G28" s="16">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="47.25">
-      <c r="A29" s="91" t="s">
-        <v>161</v>
-      </c>
-      <c r="B29" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="48" t="s">
+      <c r="A29" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D29" s="56" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="F29" s="42"/>
+      <c r="E29" s="64" t="s">
+        <v>124</v>
+      </c>
+      <c r="F29" s="53"/>
       <c r="G29" s="16">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="47.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18.75">
       <c r="A30" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C30" s="54" t="s">
-        <v>237</v>
-      </c>
-      <c r="D30" s="56" t="s">
+      <c r="B30" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="D30" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="64" t="s">
+      <c r="E30" s="41"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="16">
         <v>124</v>
       </c>
-      <c r="F30" s="53"/>
-      <c r="G30" s="16">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18.75">
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B31" s="79" t="s">
-        <v>120</v>
+      <c r="B31" s="86" t="s">
+        <v>11</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>150</v>
+        <v>230</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E31" s="41"/>
       <c r="F31" s="37"/>
       <c r="G31" s="16">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -6022,10 +6012,10 @@
         <v>147</v>
       </c>
       <c r="B32" s="86" t="s">
-        <v>11</v>
+        <v>182</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="D32" s="47" t="s">
         <v>123</v>
@@ -6033,7 +6023,7 @@
       <c r="E32" s="41"/>
       <c r="F32" s="37"/>
       <c r="G32" s="16">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -6041,10 +6031,10 @@
         <v>147</v>
       </c>
       <c r="B33" s="86" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D33" s="47" t="s">
         <v>123</v>
@@ -6052,56 +6042,56 @@
       <c r="E33" s="41"/>
       <c r="F33" s="37"/>
       <c r="G33" s="16">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18.75">
       <c r="A34" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B34" s="86" t="s">
-        <v>181</v>
+      <c r="B34" s="79" t="s">
+        <v>151</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>232</v>
+        <v>153</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E34" s="41"/>
       <c r="F34" s="37"/>
       <c r="G34" s="16">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="18.75">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="31.5">
       <c r="A35" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B35" s="79" t="s">
-        <v>151</v>
+      <c r="B35" s="86" t="s">
+        <v>280</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E35" s="41"/>
       <c r="F35" s="37"/>
       <c r="G35" s="16">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="31.5">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="86" t="s">
         <v>147</v>
       </c>
       <c r="B36" s="86" t="s">
-        <v>280</v>
+        <v>12</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D36" s="47" t="s">
         <v>123</v>
@@ -6109,26 +6099,26 @@
       <c r="E36" s="41"/>
       <c r="F36" s="37"/>
       <c r="G36" s="16">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18.75">
       <c r="A37" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B37" s="86" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="D37" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="37"/>
+      <c r="B37" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="61"/>
+      <c r="F37" s="16"/>
       <c r="G37" s="16">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18.75">
@@ -6136,10 +6126,10 @@
         <v>147</v>
       </c>
       <c r="B38" s="84" t="s">
-        <v>15</v>
+        <v>267</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D38" s="46" t="s">
         <v>122</v>
@@ -6147,136 +6137,136 @@
       <c r="E38" s="61"/>
       <c r="F38" s="16"/>
       <c r="G38" s="16">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="18.75">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="63">
       <c r="A39" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="B39" s="84" t="s">
-        <v>267</v>
-      </c>
-      <c r="C39" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D39" s="46" t="s">
+      <c r="B39" s="80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="61"/>
-      <c r="F39" s="16"/>
+      <c r="E39" s="50" t="s">
+        <v>361</v>
+      </c>
+      <c r="F39" s="42"/>
       <c r="G39" s="16">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="215" t="s">
-        <v>147</v>
-      </c>
-      <c r="B40" s="215" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="210" t="s">
-        <v>475</v>
-      </c>
-      <c r="D40" s="47" t="s">
-        <v>123</v>
-      </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="37"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" s="14" customFormat="1" ht="63">
+      <c r="A40" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B40" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="54" t="s">
+        <v>363</v>
+      </c>
+      <c r="D40" s="181" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="52"/>
       <c r="G40" s="16">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="63">
-      <c r="A41" s="86" t="s">
-        <v>147</v>
-      </c>
-      <c r="B41" s="80" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="D41" s="48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="14" customFormat="1" ht="31.5">
+      <c r="A41" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B41" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="C41" s="182" t="s">
+        <v>364</v>
+      </c>
+      <c r="D41" s="183" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="50" t="s">
-        <v>368</v>
-      </c>
-      <c r="F41" s="42"/>
+      <c r="E41" s="184"/>
+      <c r="F41" s="185"/>
       <c r="G41" s="16">
-        <v>141</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:7" s="14" customFormat="1" ht="63">
       <c r="A42" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B42" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="C42" s="182" t="s">
+        <v>366</v>
+      </c>
+      <c r="D42" s="183" t="s">
+        <v>123</v>
+      </c>
+      <c r="E42" s="184"/>
+      <c r="F42" s="185"/>
+      <c r="G42" s="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" s="14" customFormat="1" ht="18.75">
+      <c r="A43" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B43" s="186" t="s">
+        <v>367</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>368</v>
+      </c>
+      <c r="D43" s="183" t="s">
+        <v>123</v>
+      </c>
+      <c r="E43" s="187"/>
+      <c r="F43" s="188"/>
+      <c r="G43" s="16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" s="14" customFormat="1" ht="31.5">
+      <c r="A44" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B44" s="186" t="s">
         <v>369</v>
       </c>
-      <c r="B42" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="54" t="s">
+      <c r="C44" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="D42" s="181" t="s">
-        <v>122</v>
-      </c>
-      <c r="E42" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="F42" s="52"/>
-      <c r="G42" s="16">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" s="14" customFormat="1" ht="31.5">
-      <c r="A43" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B43" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="C43" s="182" t="s">
-        <v>371</v>
-      </c>
-      <c r="D43" s="183" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43" s="184"/>
-      <c r="F43" s="185"/>
-      <c r="G43" s="16">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" s="14" customFormat="1" ht="63">
-      <c r="A44" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B44" s="79" t="s">
-        <v>372</v>
-      </c>
-      <c r="C44" s="182" t="s">
-        <v>373</v>
       </c>
       <c r="D44" s="183" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="184"/>
-      <c r="F44" s="185"/>
+      <c r="E44" s="187"/>
+      <c r="F44" s="188"/>
       <c r="G44" s="16">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="14" customFormat="1" ht="63">
       <c r="A45" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B45" s="186" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D45" s="183" t="s">
         <v>123</v>
@@ -6284,56 +6274,56 @@
       <c r="E45" s="187"/>
       <c r="F45" s="188"/>
       <c r="G45" s="16">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A46" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B46" s="186" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D46" s="183" t="s">
         <v>123</v>
       </c>
-      <c r="E46" s="187"/>
-      <c r="F46" s="188"/>
+      <c r="E46" s="184"/>
+      <c r="F46" s="185"/>
       <c r="G46" s="16">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" s="14" customFormat="1" ht="63">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A47" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B47" s="186" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D47" s="183" t="s">
         <v>123</v>
       </c>
-      <c r="E47" s="187"/>
-      <c r="F47" s="188"/>
+      <c r="E47" s="184"/>
+      <c r="F47" s="185"/>
       <c r="G47" s="16">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A48" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B48" s="186" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D48" s="183" t="s">
         <v>123</v>
@@ -6341,37 +6331,39 @@
       <c r="E48" s="184"/>
       <c r="F48" s="185"/>
       <c r="G48" s="16">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A49" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B49" s="186" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D49" s="183" t="s">
         <v>123</v>
       </c>
       <c r="E49" s="184"/>
-      <c r="F49" s="185"/>
+      <c r="F49" s="185" t="s">
+        <v>146</v>
+      </c>
       <c r="G49" s="16">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A50" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B50" s="186" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D50" s="183" t="s">
         <v>123</v>
@@ -6379,172 +6371,170 @@
       <c r="E50" s="184"/>
       <c r="F50" s="185"/>
       <c r="G50" s="16">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A51" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B51" s="186" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D51" s="183" t="s">
         <v>123</v>
       </c>
       <c r="E51" s="184"/>
-      <c r="F51" s="185" t="s">
-        <v>146</v>
-      </c>
+      <c r="F51" s="185"/>
       <c r="G51" s="16">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A52" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B52" s="186" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>389</v>
-      </c>
-      <c r="D52" s="183" t="s">
-        <v>123</v>
+        <v>386</v>
+      </c>
+      <c r="D52" s="189" t="s">
+        <v>122</v>
       </c>
       <c r="E52" s="184"/>
       <c r="F52" s="185"/>
       <c r="G52" s="16">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A53" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B53" s="186" t="s">
-        <v>390</v>
+        <v>362</v>
+      </c>
+      <c r="B53" s="190" t="s">
+        <v>387</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>391</v>
-      </c>
-      <c r="D53" s="183" t="s">
-        <v>123</v>
+        <v>388</v>
+      </c>
+      <c r="D53" s="189" t="s">
+        <v>122</v>
       </c>
       <c r="E53" s="184"/>
       <c r="F53" s="185"/>
       <c r="G53" s="16">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A54" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B54" s="186" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D54" s="189" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E54" s="184"/>
       <c r="F54" s="185"/>
       <c r="G54" s="16">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A55" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B55" s="190" t="s">
+        <v>362</v>
+      </c>
+      <c r="B55" s="186" t="s">
+        <v>391</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D55" s="183" t="s">
+        <v>122</v>
+      </c>
+      <c r="E55" s="61"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" s="14" customFormat="1" ht="18.75">
+      <c r="A56" s="89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B56" s="186" t="s">
+        <v>393</v>
+      </c>
+      <c r="C56" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="C55" s="17" t="s">
-        <v>395</v>
-      </c>
-      <c r="D55" s="189" t="s">
+      <c r="D56" s="183" t="s">
         <v>122</v>
       </c>
-      <c r="E55" s="184"/>
-      <c r="F55" s="185"/>
-      <c r="G55" s="16">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" s="14" customFormat="1" ht="31.5">
-      <c r="A56" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B56" s="186" t="s">
-        <v>396</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>397</v>
-      </c>
-      <c r="D56" s="189" t="s">
-        <v>123</v>
-      </c>
-      <c r="E56" s="184"/>
-      <c r="F56" s="185"/>
+      <c r="E56" s="61"/>
+      <c r="F56" s="16"/>
       <c r="G56" s="16">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A57" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B57" s="186" t="s">
-        <v>398</v>
+        <v>362</v>
+      </c>
+      <c r="B57" s="190" t="s">
+        <v>15</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>399</v>
-      </c>
-      <c r="D57" s="183" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" s="46" t="s">
         <v>122</v>
       </c>
       <c r="E57" s="61"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A58" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B58" s="186" t="s">
-        <v>400</v>
+        <v>362</v>
+      </c>
+      <c r="B58" s="190" t="s">
+        <v>267</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>401</v>
-      </c>
-      <c r="D58" s="183" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="46" t="s">
         <v>122</v>
       </c>
       <c r="E58" s="61"/>
       <c r="F58" s="16"/>
       <c r="G58" s="16">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A59" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B59" s="190" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D59" s="46" t="s">
         <v>122</v>
@@ -6552,174 +6542,174 @@
       <c r="E59" s="61"/>
       <c r="F59" s="16"/>
       <c r="G59" s="16">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A60" s="89" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B60" s="190" t="s">
-        <v>267</v>
+        <v>14</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D60" s="46" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E60" s="61"/>
       <c r="F60" s="16"/>
       <c r="G60" s="16">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A61" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B61" s="190" t="s">
-        <v>266</v>
+        <v>362</v>
+      </c>
+      <c r="B61" s="186" t="s">
+        <v>395</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D61" s="46" t="s">
+        <v>396</v>
+      </c>
+      <c r="D61" s="189" t="s">
         <v>122</v>
       </c>
       <c r="E61" s="61"/>
       <c r="F61" s="16"/>
       <c r="G61" s="16">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A62" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B62" s="190" t="s">
-        <v>14</v>
+        <v>362</v>
+      </c>
+      <c r="B62" s="186" t="s">
+        <v>397</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="D62" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="D62" s="189" t="s">
         <v>123</v>
       </c>
       <c r="E62" s="61"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A63" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B63" s="186" t="s">
+        <v>362</v>
+      </c>
+      <c r="B63" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="51" t="s">
+        <v>399</v>
+      </c>
+      <c r="D63" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E63" s="63" t="s">
+        <v>400</v>
+      </c>
+      <c r="F63" s="42"/>
+      <c r="G63" s="16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="14" customFormat="1" ht="47.25">
+      <c r="A64" s="191" t="s">
         <v>402</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="B64" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C64" s="54" t="s">
         <v>403</v>
       </c>
-      <c r="D63" s="189" t="s">
+      <c r="D64" s="181" t="s">
         <v>122</v>
       </c>
-      <c r="E63" s="61"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" s="14" customFormat="1" ht="18.75">
-      <c r="A64" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B64" s="186" t="s">
+      <c r="E64" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F64" s="53"/>
+      <c r="G64" s="16">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="14" customFormat="1" ht="18.75">
+      <c r="A65" s="191" t="s">
+        <v>402</v>
+      </c>
+      <c r="B65" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="C65" s="192" t="s">
         <v>404</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="D65" s="193" t="s">
+        <v>122</v>
+      </c>
+      <c r="E65" s="194"/>
+      <c r="F65" s="195"/>
+      <c r="G65" s="16">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" s="14" customFormat="1" ht="18.75">
+      <c r="A66" s="191" t="s">
+        <v>402</v>
+      </c>
+      <c r="B66" s="196" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="192" t="s">
         <v>405</v>
       </c>
-      <c r="D64" s="189" t="s">
+      <c r="D66" s="193" t="s">
         <v>123</v>
       </c>
-      <c r="E64" s="61"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="16">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" s="14" customFormat="1" ht="47.25">
-      <c r="A65" s="89" t="s">
-        <v>369</v>
-      </c>
-      <c r="B65" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" s="51" t="s">
-        <v>406</v>
-      </c>
-      <c r="D65" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="E65" s="63" t="s">
-        <v>407</v>
-      </c>
-      <c r="F65" s="42"/>
-      <c r="G65" s="16">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" s="14" customFormat="1" ht="47.25">
-      <c r="A66" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B66" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="54" t="s">
-        <v>410</v>
-      </c>
-      <c r="D66" s="181" t="s">
-        <v>122</v>
-      </c>
-      <c r="E66" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="F66" s="53"/>
+      <c r="E66" s="194"/>
+      <c r="F66" s="195"/>
       <c r="G66" s="16">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A67" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B67" s="79" t="s">
-        <v>120</v>
+        <v>402</v>
+      </c>
+      <c r="B67" s="196" t="s">
+        <v>7</v>
       </c>
       <c r="C67" s="192" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D67" s="193" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E67" s="194"/>
       <c r="F67" s="195"/>
       <c r="G67" s="16">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A68" s="191" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B68" s="196" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C68" s="192" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D68" s="193" t="s">
         <v>123</v>
@@ -6727,18 +6717,18 @@
       <c r="E68" s="194"/>
       <c r="F68" s="195"/>
       <c r="G68" s="16">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A69" s="191" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B69" s="196" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C69" s="192" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="D69" s="193" t="s">
         <v>123</v>
@@ -6746,56 +6736,56 @@
       <c r="E69" s="194"/>
       <c r="F69" s="195"/>
       <c r="G69" s="16">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A70" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B70" s="196" t="s">
-        <v>13</v>
-      </c>
-      <c r="C70" s="192" t="s">
-        <v>414</v>
-      </c>
-      <c r="D70" s="193" t="s">
-        <v>123</v>
+        <v>402</v>
+      </c>
+      <c r="B70" s="190" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D70" s="197" t="s">
+        <v>122</v>
       </c>
       <c r="E70" s="194"/>
       <c r="F70" s="195"/>
       <c r="G70" s="16">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A71" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B71" s="196" t="s">
-        <v>12</v>
-      </c>
-      <c r="C71" s="192" t="s">
-        <v>415</v>
-      </c>
-      <c r="D71" s="193" t="s">
-        <v>123</v>
+        <v>402</v>
+      </c>
+      <c r="B71" s="190" t="s">
+        <v>267</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="197" t="s">
+        <v>122</v>
       </c>
       <c r="E71" s="194"/>
       <c r="F71" s="195"/>
       <c r="G71" s="16">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A72" s="191" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B72" s="190" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="C72" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D72" s="197" t="s">
         <v>122</v>
@@ -6803,136 +6793,136 @@
       <c r="E72" s="194"/>
       <c r="F72" s="195"/>
       <c r="G72" s="16">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A73" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B73" s="190" t="s">
-        <v>267</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>127</v>
+        <v>402</v>
+      </c>
+      <c r="B73" s="196" t="s">
+        <v>14</v>
+      </c>
+      <c r="C73" s="192" t="s">
+        <v>129</v>
       </c>
       <c r="D73" s="197" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E73" s="194"/>
       <c r="F73" s="195"/>
       <c r="G73" s="16">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A74" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B74" s="190" t="s">
-        <v>266</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D74" s="197" t="s">
+        <v>402</v>
+      </c>
+      <c r="B74" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D74" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="E74" s="194"/>
-      <c r="F74" s="195"/>
+      <c r="E74" s="50" t="s">
+        <v>183</v>
+      </c>
+      <c r="F74" s="42"/>
       <c r="G74" s="16">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:7" s="14" customFormat="1" ht="18.75">
-      <c r="A75" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B75" s="196" t="s">
-        <v>14</v>
-      </c>
-      <c r="C75" s="192" t="s">
-        <v>129</v>
-      </c>
-      <c r="D75" s="197" t="s">
-        <v>123</v>
-      </c>
-      <c r="E75" s="194"/>
-      <c r="F75" s="195"/>
+      <c r="A75" s="198" t="s">
+        <v>415</v>
+      </c>
+      <c r="B75" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="C75" s="54" t="s">
+        <v>416</v>
+      </c>
+      <c r="D75" s="181" t="s">
+        <v>122</v>
+      </c>
+      <c r="E75" s="60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F75" s="53"/>
       <c r="G75" s="16">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" s="14" customFormat="1" ht="47.25">
-      <c r="A76" s="191" t="s">
-        <v>409</v>
-      </c>
-      <c r="B76" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" s="51" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76" s="48" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" s="14" customFormat="1" ht="31.5">
+      <c r="A76" s="198" t="s">
+        <v>415</v>
+      </c>
+      <c r="B76" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="D76" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="E76" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="F76" s="42"/>
+      <c r="E76" s="60"/>
+      <c r="F76" s="53"/>
       <c r="G76" s="16">
-        <v>168</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A77" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B77" s="78" t="s">
-        <v>0</v>
-      </c>
-      <c r="C77" s="54" t="s">
-        <v>423</v>
-      </c>
-      <c r="D77" s="181" t="s">
-        <v>122</v>
-      </c>
-      <c r="E77" s="60" t="s">
-        <v>124</v>
-      </c>
-      <c r="F77" s="53"/>
+        <v>415</v>
+      </c>
+      <c r="B77" s="81" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D77" s="49" t="s">
+        <v>123</v>
+      </c>
+      <c r="E77" s="61"/>
+      <c r="F77" s="16"/>
       <c r="G77" s="16">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A78" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B78" s="79" t="s">
-        <v>120</v>
+        <v>415</v>
+      </c>
+      <c r="B78" s="81" t="s">
+        <v>12</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="D78" s="49" t="s">
-        <v>122</v>
-      </c>
-      <c r="E78" s="60"/>
-      <c r="F78" s="53"/>
+        <v>123</v>
+      </c>
+      <c r="E78" s="61"/>
+      <c r="F78" s="16"/>
       <c r="G78" s="16">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A79" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B79" s="81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>166</v>
+        <v>419</v>
       </c>
       <c r="D79" s="49" t="s">
         <v>123</v>
@@ -6940,18 +6930,18 @@
       <c r="E79" s="61"/>
       <c r="F79" s="16"/>
       <c r="G79" s="16">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="80" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A80" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B80" s="81" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D80" s="49" t="s">
         <v>123</v>
@@ -6959,75 +6949,75 @@
       <c r="E80" s="61"/>
       <c r="F80" s="16"/>
       <c r="G80" s="16">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A81" s="198" t="s">
+        <v>415</v>
+      </c>
+      <c r="B81" s="199" t="s">
+        <v>421</v>
+      </c>
+      <c r="C81" s="200" t="s">
         <v>422</v>
       </c>
-      <c r="B81" s="81" t="s">
-        <v>11</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>426</v>
-      </c>
       <c r="D81" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E81" s="61"/>
       <c r="F81" s="16"/>
       <c r="G81" s="16">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A82" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B82" s="81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>427</v>
+        <v>415</v>
+      </c>
+      <c r="B82" s="199" t="s">
+        <v>423</v>
+      </c>
+      <c r="C82" s="200" t="s">
+        <v>424</v>
       </c>
       <c r="D82" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82" s="61"/>
       <c r="F82" s="16"/>
       <c r="G82" s="16">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" s="14" customFormat="1" ht="47.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" s="14" customFormat="1" ht="78.75">
       <c r="A83" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B83" s="199" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C83" s="200" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D83" s="49" t="s">
-        <v>122</v>
+        <v>427</v>
       </c>
       <c r="E83" s="61"/>
       <c r="F83" s="16"/>
       <c r="G83" s="16">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="84" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A84" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B84" s="199" t="s">
-        <v>430</v>
-      </c>
-      <c r="C84" s="200" t="s">
-        <v>431</v>
+        <v>415</v>
+      </c>
+      <c r="B84" s="201" t="s">
+        <v>428</v>
+      </c>
+      <c r="C84" s="202" t="s">
+        <v>429</v>
       </c>
       <c r="D84" s="49" t="s">
         <v>122</v>
@@ -7035,37 +7025,37 @@
       <c r="E84" s="61"/>
       <c r="F84" s="16"/>
       <c r="G84" s="16">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" s="14" customFormat="1" ht="78.75">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A85" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B85" s="199" t="s">
-        <v>432</v>
-      </c>
-      <c r="C85" s="200" t="s">
-        <v>433</v>
+        <v>415</v>
+      </c>
+      <c r="B85" s="201" t="s">
+        <v>430</v>
+      </c>
+      <c r="C85" s="202" t="s">
+        <v>431</v>
       </c>
       <c r="D85" s="49" t="s">
-        <v>434</v>
+        <v>122</v>
       </c>
       <c r="E85" s="61"/>
       <c r="F85" s="16"/>
       <c r="G85" s="16">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="86" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A86" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B86" s="201" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C86" s="202" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D86" s="49" t="s">
         <v>122</v>
@@ -7073,18 +7063,18 @@
       <c r="E86" s="61"/>
       <c r="F86" s="16"/>
       <c r="G86" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" s="14" customFormat="1" ht="47.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A87" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B87" s="201" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C87" s="202" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D87" s="49" t="s">
         <v>122</v>
@@ -7092,113 +7082,113 @@
       <c r="E87" s="61"/>
       <c r="F87" s="16"/>
       <c r="G87" s="16">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A88" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B88" s="201" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C88" s="202" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D88" s="49" t="s">
-        <v>122</v>
+        <v>427</v>
       </c>
       <c r="E88" s="61"/>
       <c r="F88" s="16"/>
       <c r="G88" s="16">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A89" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B89" s="201" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C89" s="202" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D89" s="49" t="s">
-        <v>122</v>
+        <v>427</v>
       </c>
       <c r="E89" s="61"/>
       <c r="F89" s="16"/>
       <c r="G89" s="16">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="90" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A90" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B90" s="201" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C90" s="202" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D90" s="49" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E90" s="61"/>
       <c r="F90" s="16"/>
       <c r="G90" s="16">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" s="14" customFormat="1" ht="47.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A91" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B91" s="201" t="s">
-        <v>445</v>
-      </c>
-      <c r="C91" s="202" t="s">
-        <v>446</v>
-      </c>
-      <c r="D91" s="49" t="s">
-        <v>434</v>
+        <v>415</v>
+      </c>
+      <c r="B91" s="203" t="s">
+        <v>442</v>
+      </c>
+      <c r="C91" s="182" t="s">
+        <v>443</v>
+      </c>
+      <c r="D91" s="204" t="s">
+        <v>122</v>
       </c>
       <c r="E91" s="61"/>
       <c r="F91" s="16"/>
       <c r="G91" s="16">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" s="14" customFormat="1" ht="47.25">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A92" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B92" s="201" t="s">
-        <v>447</v>
-      </c>
-      <c r="C92" s="202" t="s">
-        <v>448</v>
-      </c>
-      <c r="D92" s="49" t="s">
-        <v>434</v>
+        <v>415</v>
+      </c>
+      <c r="B92" s="203" t="s">
+        <v>444</v>
+      </c>
+      <c r="C92" s="182" t="s">
+        <v>445</v>
+      </c>
+      <c r="D92" s="204" t="s">
+        <v>122</v>
       </c>
       <c r="E92" s="61"/>
       <c r="F92" s="16"/>
       <c r="G92" s="16">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A93" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B93" s="203" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C93" s="182" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D93" s="204" t="s">
         <v>122</v>
@@ -7206,18 +7196,18 @@
       <c r="E93" s="61"/>
       <c r="F93" s="16"/>
       <c r="G93" s="16">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" s="14" customFormat="1" ht="31.5">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A94" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B94" s="203" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C94" s="182" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D94" s="204" t="s">
         <v>122</v>
@@ -7225,132 +7215,132 @@
       <c r="E94" s="61"/>
       <c r="F94" s="16"/>
       <c r="G94" s="16">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="95" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A95" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B95" s="203" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C95" s="182" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D95" s="204" t="s">
-        <v>122</v>
+        <v>427</v>
       </c>
       <c r="E95" s="61"/>
       <c r="F95" s="16"/>
       <c r="G95" s="16">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="96" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A96" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B96" s="203" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C96" s="182" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D96" s="204" t="s">
-        <v>122</v>
+        <v>427</v>
       </c>
       <c r="E96" s="61"/>
       <c r="F96" s="16"/>
       <c r="G96" s="16">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="97" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A97" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B97" s="203" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C97" s="182" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D97" s="204" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E97" s="61"/>
       <c r="F97" s="16"/>
       <c r="G97" s="16">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" s="14" customFormat="1" ht="47.25">
       <c r="A98" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B98" s="203" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C98" s="182" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D98" s="204" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="E98" s="61"/>
       <c r="F98" s="16"/>
       <c r="G98" s="16">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="99" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A99" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B99" s="203" t="s">
-        <v>461</v>
-      </c>
-      <c r="C99" s="182" t="s">
-        <v>462</v>
-      </c>
-      <c r="D99" s="204" t="s">
-        <v>434</v>
+        <v>415</v>
+      </c>
+      <c r="B99" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D99" s="49" t="s">
+        <v>122</v>
       </c>
       <c r="E99" s="61"/>
       <c r="F99" s="16"/>
       <c r="G99" s="16">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" s="14" customFormat="1" ht="47.25">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A100" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B100" s="203" t="s">
-        <v>463</v>
-      </c>
-      <c r="C100" s="182" t="s">
-        <v>464</v>
-      </c>
-      <c r="D100" s="204" t="s">
-        <v>434</v>
+        <v>415</v>
+      </c>
+      <c r="B100" s="190" t="s">
+        <v>15</v>
+      </c>
+      <c r="C100" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="D100" s="49" t="s">
+        <v>122</v>
       </c>
       <c r="E100" s="61"/>
       <c r="F100" s="16"/>
       <c r="G100" s="16">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="101" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A101" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B101" s="44" t="s">
-        <v>8</v>
+        <v>415</v>
+      </c>
+      <c r="B101" s="190" t="s">
+        <v>267</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>178</v>
+        <v>127</v>
       </c>
       <c r="D101" s="49" t="s">
         <v>122</v>
@@ -7358,18 +7348,18 @@
       <c r="E101" s="61"/>
       <c r="F101" s="16"/>
       <c r="G101" s="16">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="102" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A102" s="198" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B102" s="190" t="s">
-        <v>15</v>
+        <v>266</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D102" s="49" t="s">
         <v>122</v>
@@ -7377,108 +7367,70 @@
       <c r="E102" s="61"/>
       <c r="F102" s="16"/>
       <c r="G102" s="16">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="103" spans="1:7" s="14" customFormat="1" ht="18.75">
       <c r="A103" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B103" s="190" t="s">
-        <v>267</v>
+        <v>415</v>
+      </c>
+      <c r="B103" s="44" t="s">
+        <v>14</v>
       </c>
       <c r="C103" s="17" t="s">
-        <v>127</v>
+        <v>458</v>
       </c>
       <c r="D103" s="49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E103" s="61"/>
       <c r="F103" s="16"/>
       <c r="G103" s="16">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" s="14" customFormat="1" ht="31.5">
       <c r="A104" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B104" s="190" t="s">
-        <v>266</v>
+        <v>415</v>
+      </c>
+      <c r="B104" s="44" t="s">
+        <v>459</v>
       </c>
       <c r="C104" s="17" t="s">
-        <v>126</v>
+        <v>460</v>
       </c>
       <c r="D104" s="49" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E104" s="61"/>
       <c r="F104" s="16"/>
       <c r="G104" s="16">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" s="14" customFormat="1" ht="18.75">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="14" customFormat="1" ht="126">
       <c r="A105" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B105" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C105" s="17" t="s">
-        <v>465</v>
-      </c>
-      <c r="D105" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="E105" s="61"/>
-      <c r="F105" s="16"/>
+        <v>415</v>
+      </c>
+      <c r="B105" s="81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="51" t="s">
+        <v>461</v>
+      </c>
+      <c r="D105" s="48" t="s">
+        <v>122</v>
+      </c>
+      <c r="E105" s="205" t="s">
+        <v>462</v>
+      </c>
+      <c r="F105" s="42"/>
       <c r="G105" s="16">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" s="14" customFormat="1" ht="31.5">
-      <c r="A106" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B106" s="44" t="s">
-        <v>466</v>
-      </c>
-      <c r="C106" s="17" t="s">
-        <v>467</v>
-      </c>
-      <c r="D106" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="E106" s="61"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="16">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" s="14" customFormat="1" ht="126">
-      <c r="A107" s="198" t="s">
-        <v>422</v>
-      </c>
-      <c r="B107" s="81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C107" s="51" t="s">
-        <v>468</v>
-      </c>
-      <c r="D107" s="48" t="s">
-        <v>122</v>
-      </c>
-      <c r="E107" s="205" t="s">
-        <v>469</v>
-      </c>
-      <c r="F107" s="42"/>
-      <c r="G107" s="16">
         <v>386</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G39" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -7489,7 +7441,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -7549,10 +7501,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>88</v>
@@ -7575,7 +7527,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
@@ -7634,58 +7586,58 @@
         <v>7</v>
       </c>
       <c r="G1" s="199" t="s">
+        <v>421</v>
+      </c>
+      <c r="H1" s="199" t="s">
+        <v>423</v>
+      </c>
+      <c r="I1" s="199" t="s">
+        <v>425</v>
+      </c>
+      <c r="J1" s="201" t="s">
         <v>428</v>
       </c>
-      <c r="H1" s="199" t="s">
+      <c r="K1" s="201" t="s">
         <v>430</v>
       </c>
-      <c r="I1" s="199" t="s">
+      <c r="L1" s="201" t="s">
         <v>432</v>
       </c>
-      <c r="J1" s="201" t="s">
-        <v>435</v>
-      </c>
-      <c r="K1" s="201" t="s">
-        <v>437</v>
-      </c>
-      <c r="L1" s="201" t="s">
-        <v>439</v>
-      </c>
       <c r="M1" s="201" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="N1" s="201" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="O1" s="201" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="P1" s="201" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="Q1" s="203" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="R1" s="203" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="S1" s="203" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="T1" s="203" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="U1" s="203" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="V1" s="203" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="W1" s="203" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="X1" s="203" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="Y1" s="44" t="s">
         <v>8</v>
@@ -7703,7 +7655,7 @@
         <v>14</v>
       </c>
       <c r="AD1" s="44" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="AE1" s="81" t="s">
         <v>9</v>
@@ -7723,10 +7675,10 @@
         <v>43769</v>
       </c>
       <c r="E2" s="92" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="F2" s="92" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="G2" s="92"/>
       <c r="H2" s="92"/>
@@ -7755,7 +7707,7 @@
       </c>
       <c r="AB2" s="92"/>
       <c r="AC2" s="92" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="AD2" s="92"/>
       <c r="AE2" s="92"/>
@@ -7905,54 +7857,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75">
-      <c r="A1" s="229" t="s">
-        <v>321</v>
-      </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="229"/>
-      <c r="L1" s="229"/>
-      <c r="M1" s="229"/>
-      <c r="N1" s="229"/>
+      <c r="A1" s="222" t="s">
+        <v>319</v>
+      </c>
+      <c r="B1" s="222"/>
+      <c r="C1" s="222"/>
+      <c r="D1" s="222"/>
+      <c r="E1" s="222"/>
+      <c r="F1" s="222"/>
+      <c r="G1" s="222"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="222"/>
+      <c r="J1" s="222"/>
+      <c r="K1" s="222"/>
+      <c r="L1" s="222"/>
+      <c r="M1" s="222"/>
+      <c r="N1" s="222"/>
     </row>
     <row r="2" spans="1:14" ht="25.5">
-      <c r="A2" s="216" t="s">
-        <v>322</v>
-      </c>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
-      <c r="K2" s="216"/>
-      <c r="L2" s="216"/>
-      <c r="M2" s="216"/>
-      <c r="N2" s="216"/>
+      <c r="A2" s="218" t="s">
+        <v>320</v>
+      </c>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
+      <c r="J2" s="218"/>
+      <c r="K2" s="218"/>
+      <c r="L2" s="218"/>
+      <c r="M2" s="218"/>
+      <c r="N2" s="218"/>
     </row>
     <row r="3" spans="1:14" ht="15.75">
       <c r="A3" s="121"/>
       <c r="B3" s="121"/>
       <c r="C3" s="121"/>
-      <c r="D3" s="230" t="s">
-        <v>323</v>
-      </c>
-      <c r="E3" s="230"/>
-      <c r="F3" s="230"/>
-      <c r="G3" s="230"/>
-      <c r="H3" s="230"/>
-      <c r="I3" s="230"/>
-      <c r="J3" s="230"/>
+      <c r="D3" s="223" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="223"/>
+      <c r="F3" s="223"/>
+      <c r="G3" s="223"/>
+      <c r="H3" s="223"/>
+      <c r="I3" s="223"/>
+      <c r="J3" s="223"/>
       <c r="K3" s="122"/>
       <c r="L3" s="123"/>
       <c r="M3" s="123"/>
@@ -7974,50 +7926,50 @@
     </row>
     <row r="5" spans="1:14" s="127" customFormat="1" ht="78.75">
       <c r="A5" s="124" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" s="125" t="s">
+        <v>323</v>
+      </c>
+      <c r="C5" s="124" t="s">
         <v>324</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="D5" s="125" t="s">
         <v>325</v>
       </c>
-      <c r="C5" s="124" t="s">
+      <c r="E5" s="126" t="s">
         <v>326</v>
       </c>
-      <c r="D5" s="125" t="s">
+      <c r="F5" s="126" t="s">
+        <v>334</v>
+      </c>
+      <c r="G5" s="125" t="s">
         <v>327</v>
       </c>
-      <c r="E5" s="126" t="s">
+      <c r="H5" s="125" t="s">
         <v>328</v>
-      </c>
-      <c r="F5" s="126" t="s">
-        <v>336</v>
-      </c>
-      <c r="G5" s="125" t="s">
-        <v>329</v>
-      </c>
-      <c r="H5" s="125" t="s">
-        <v>330</v>
       </c>
       <c r="I5" s="126" t="s">
         <v>177</v>
       </c>
       <c r="J5" s="126" t="s">
+        <v>329</v>
+      </c>
+      <c r="K5" s="126" t="s">
+        <v>330</v>
+      </c>
+      <c r="L5" s="126" t="s">
         <v>331</v>
       </c>
-      <c r="K5" s="126" t="s">
+      <c r="M5" s="126" t="s">
         <v>332</v>
       </c>
-      <c r="L5" s="126" t="s">
-        <v>333</v>
-      </c>
-      <c r="M5" s="126" t="s">
-        <v>334</v>
-      </c>
     </row>
     <row r="6" spans="1:14" s="127" customFormat="1" ht="30" customHeight="1">
-      <c r="A6" s="231" t="s">
+      <c r="A6" s="224" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="224">
+      <c r="B6" s="226">
         <v>0.2</v>
       </c>
       <c r="C6" s="173" t="s">
@@ -8052,8 +8004,8 @@
       <c r="M6" s="130"/>
     </row>
     <row r="7" spans="1:14" s="127" customFormat="1" ht="30" customHeight="1">
-      <c r="A7" s="232"/>
-      <c r="B7" s="225"/>
+      <c r="A7" s="225"/>
+      <c r="B7" s="227"/>
       <c r="C7" s="174"/>
       <c r="D7" s="167"/>
       <c r="E7" s="19" t="s">
@@ -8082,8 +8034,8 @@
       <c r="M7" s="130"/>
     </row>
     <row r="8" spans="1:14" s="127" customFormat="1" ht="31.5">
-      <c r="A8" s="232"/>
-      <c r="B8" s="225"/>
+      <c r="A8" s="225"/>
+      <c r="B8" s="227"/>
       <c r="C8" s="175" t="s">
         <v>17</v>
       </c>
@@ -8116,8 +8068,8 @@
       <c r="M8" s="130"/>
     </row>
     <row r="9" spans="1:14" s="127" customFormat="1" ht="31.5">
-      <c r="A9" s="232"/>
-      <c r="B9" s="225"/>
+      <c r="A9" s="225"/>
+      <c r="B9" s="227"/>
       <c r="C9" s="176"/>
       <c r="D9" s="161"/>
       <c r="E9" s="19" t="s">
@@ -8146,10 +8098,10 @@
       <c r="M9" s="134"/>
     </row>
     <row r="10" spans="1:14" ht="31.5">
-      <c r="A10" s="223" t="s">
+      <c r="A10" s="231" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="224">
+      <c r="B10" s="226">
         <v>0.25</v>
       </c>
       <c r="C10" s="168" t="s">
@@ -8182,8 +8134,8 @@
       <c r="M10" s="136"/>
     </row>
     <row r="11" spans="1:14" ht="31.5">
-      <c r="A11" s="223"/>
-      <c r="B11" s="225"/>
+      <c r="A11" s="231"/>
+      <c r="B11" s="227"/>
       <c r="C11" s="169"/>
       <c r="D11" s="167"/>
       <c r="E11" s="20" t="s">
@@ -8210,10 +8162,10 @@
       <c r="M11" s="136"/>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1">
-      <c r="A12" s="226" t="s">
-        <v>335</v>
-      </c>
-      <c r="B12" s="224">
+      <c r="A12" s="232" t="s">
+        <v>333</v>
+      </c>
+      <c r="B12" s="226">
         <v>0.45</v>
       </c>
       <c r="C12" s="158" t="s">
@@ -8246,8 +8198,8 @@
       <c r="M12" s="139"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A13" s="227"/>
-      <c r="B13" s="225"/>
+      <c r="A13" s="233"/>
+      <c r="B13" s="227"/>
       <c r="C13" s="170" t="s">
         <v>20</v>
       </c>
@@ -8278,8 +8230,8 @@
       <c r="M13" s="139"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1">
-      <c r="A14" s="227"/>
-      <c r="B14" s="225"/>
+      <c r="A14" s="233"/>
+      <c r="B14" s="227"/>
       <c r="C14" s="171"/>
       <c r="D14" s="166"/>
       <c r="E14" s="21" t="s">
@@ -8306,8 +8258,8 @@
       <c r="M14" s="139"/>
     </row>
     <row r="15" spans="1:14" ht="31.5">
-      <c r="A15" s="227"/>
-      <c r="B15" s="225"/>
+      <c r="A15" s="233"/>
+      <c r="B15" s="227"/>
       <c r="C15" s="171"/>
       <c r="D15" s="166"/>
       <c r="E15" s="21" t="s">
@@ -8334,8 +8286,8 @@
       <c r="M15" s="139"/>
     </row>
     <row r="16" spans="1:14" ht="31.5">
-      <c r="A16" s="227"/>
-      <c r="B16" s="225"/>
+      <c r="A16" s="233"/>
+      <c r="B16" s="227"/>
       <c r="C16" s="172"/>
       <c r="D16" s="167"/>
       <c r="E16" s="21" t="s">
@@ -8362,8 +8314,8 @@
       <c r="M16" s="139"/>
     </row>
     <row r="17" spans="1:13" ht="31.5">
-      <c r="A17" s="227"/>
-      <c r="B17" s="225"/>
+      <c r="A17" s="233"/>
+      <c r="B17" s="227"/>
       <c r="C17" s="170" t="s">
         <v>21</v>
       </c>
@@ -8394,8 +8346,8 @@
       <c r="M17" s="139"/>
     </row>
     <row r="18" spans="1:13" ht="15.75">
-      <c r="A18" s="227"/>
-      <c r="B18" s="225"/>
+      <c r="A18" s="233"/>
+      <c r="B18" s="227"/>
       <c r="C18" s="171"/>
       <c r="D18" s="166"/>
       <c r="E18" s="21" t="s">
@@ -8422,8 +8374,8 @@
       <c r="M18" s="139"/>
     </row>
     <row r="19" spans="1:13" ht="74.25" customHeight="1">
-      <c r="A19" s="227"/>
-      <c r="B19" s="225"/>
+      <c r="A19" s="233"/>
+      <c r="B19" s="227"/>
       <c r="C19" s="172"/>
       <c r="D19" s="167"/>
       <c r="E19" s="21" t="s">
@@ -8450,8 +8402,8 @@
       <c r="M19" s="139"/>
     </row>
     <row r="20" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A20" s="227"/>
-      <c r="B20" s="225"/>
+      <c r="A20" s="233"/>
+      <c r="B20" s="227"/>
       <c r="C20" s="170" t="s">
         <v>22</v>
       </c>
@@ -8482,8 +8434,8 @@
       <c r="M20" s="139"/>
     </row>
     <row r="21" spans="1:13" ht="31.5">
-      <c r="A21" s="227"/>
-      <c r="B21" s="225"/>
+      <c r="A21" s="233"/>
+      <c r="B21" s="227"/>
       <c r="C21" s="171"/>
       <c r="D21" s="166"/>
       <c r="E21" s="22" t="s">
@@ -8510,8 +8462,8 @@
       <c r="M21" s="139"/>
     </row>
     <row r="22" spans="1:13" ht="31.5">
-      <c r="A22" s="227"/>
-      <c r="B22" s="225"/>
+      <c r="A22" s="233"/>
+      <c r="B22" s="227"/>
       <c r="C22" s="171"/>
       <c r="D22" s="166"/>
       <c r="E22" s="22" t="s">
@@ -8538,8 +8490,8 @@
       <c r="M22" s="140"/>
     </row>
     <row r="23" spans="1:13" ht="31.5">
-      <c r="A23" s="227"/>
-      <c r="B23" s="225"/>
+      <c r="A23" s="233"/>
+      <c r="B23" s="227"/>
       <c r="C23" s="171"/>
       <c r="D23" s="166"/>
       <c r="E23" s="21" t="s">
@@ -8566,8 +8518,8 @@
       <c r="M23" s="140"/>
     </row>
     <row r="24" spans="1:13" ht="31.5">
-      <c r="A24" s="227"/>
-      <c r="B24" s="228"/>
+      <c r="A24" s="233"/>
+      <c r="B24" s="234"/>
       <c r="C24" s="172"/>
       <c r="D24" s="167"/>
       <c r="E24" s="21" t="s">
@@ -8594,10 +8546,10 @@
       <c r="M24" s="140"/>
     </row>
     <row r="25" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A25" s="220" t="s">
+      <c r="A25" s="228" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="222">
+      <c r="B25" s="230">
         <v>0.1</v>
       </c>
       <c r="C25" s="162" t="s">
@@ -8630,8 +8582,8 @@
       <c r="M25" s="142"/>
     </row>
     <row r="26" spans="1:13" ht="31.5">
-      <c r="A26" s="221"/>
-      <c r="B26" s="222"/>
+      <c r="A26" s="229"/>
+      <c r="B26" s="230"/>
       <c r="C26" s="163"/>
       <c r="D26" s="166"/>
       <c r="E26" s="23" t="s">
@@ -8658,8 +8610,8 @@
       <c r="M26" s="142"/>
     </row>
     <row r="27" spans="1:13" ht="47.25">
-      <c r="A27" s="221"/>
-      <c r="B27" s="222"/>
+      <c r="A27" s="229"/>
+      <c r="B27" s="230"/>
       <c r="C27" s="163"/>
       <c r="D27" s="166"/>
       <c r="E27" s="24" t="s">
@@ -8686,8 +8638,8 @@
       <c r="M27" s="142"/>
     </row>
     <row r="28" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A28" s="221"/>
-      <c r="B28" s="222"/>
+      <c r="A28" s="229"/>
+      <c r="B28" s="230"/>
       <c r="C28" s="163"/>
       <c r="D28" s="166"/>
       <c r="E28" s="24" t="s">
@@ -8714,8 +8666,8 @@
       <c r="M28" s="142"/>
     </row>
     <row r="29" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A29" s="221"/>
-      <c r="B29" s="222"/>
+      <c r="A29" s="229"/>
+      <c r="B29" s="230"/>
       <c r="C29" s="164"/>
       <c r="D29" s="167"/>
       <c r="E29" s="24" t="s">
@@ -8742,8 +8694,8 @@
       <c r="M29" s="144"/>
     </row>
     <row r="30" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A30" s="221"/>
-      <c r="B30" s="222"/>
+      <c r="A30" s="229"/>
+      <c r="B30" s="230"/>
       <c r="C30" s="156" t="s">
         <v>24</v>
       </c>
@@ -8774,8 +8726,8 @@
       <c r="M30" s="144"/>
     </row>
     <row r="31" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A31" s="221"/>
-      <c r="B31" s="222"/>
+      <c r="A31" s="229"/>
+      <c r="B31" s="230"/>
       <c r="C31" s="162" t="s">
         <v>25</v>
       </c>
@@ -8806,8 +8758,8 @@
       <c r="M31" s="144"/>
     </row>
     <row r="32" spans="1:13" ht="31.5" customHeight="1">
-      <c r="A32" s="221"/>
-      <c r="B32" s="222"/>
+      <c r="A32" s="229"/>
+      <c r="B32" s="230"/>
       <c r="C32" s="164"/>
       <c r="D32" s="167"/>
       <c r="E32" s="24" t="s">
@@ -8948,17 +8900,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
     <mergeCell ref="A25:A32"/>
     <mergeCell ref="B25:B32"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A12:A24"/>
     <mergeCell ref="B12:B24"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <conditionalFormatting sqref="B6 B33:B64 B25 G12:H64 D17:D64 G6:H10 D10:D13 B10:B12">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
@@ -9001,53 +8953,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
-      <c r="A1" s="216" t="s">
+      <c r="A1" s="218" t="s">
+        <v>284</v>
+      </c>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
+    </row>
+    <row r="2" spans="1:10" ht="21">
+      <c r="A2" s="219" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75">
+      <c r="A3" s="220" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
-    </row>
-    <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="217" t="s">
-        <v>287</v>
-      </c>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="217"/>
-      <c r="J2" s="217"/>
-    </row>
-    <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="218" t="s">
-        <v>288</v>
-      </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="218"/>
-      <c r="I3" s="218"/>
-      <c r="J3" s="218"/>
+      <c r="B3" s="220"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="220"/>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
     </row>
     <row r="5" spans="1:10" ht="55.5" customHeight="1">
       <c r="A5" s="76" t="s">
         <v>279</v>
       </c>
       <c r="B5" s="76" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C5" s="76" t="s">
         <v>273</v>
@@ -9056,7 +9008,7 @@
         <v>177</v>
       </c>
       <c r="E5" s="76" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F5" s="77" t="s">
         <v>274</v>
@@ -9112,7 +9064,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="89" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B8" s="113" t="s">
         <v>26</v>
@@ -9146,7 +9098,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="89" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B9" s="113" t="s">
         <v>27</v>
@@ -9183,7 +9135,7 @@
         <v>1.2</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C10" s="98">
         <v>0.1</v>
@@ -9198,7 +9150,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="116" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B11" s="113" t="s">
         <v>28</v>
@@ -9232,7 +9184,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="116" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B12" s="113" t="s">
         <v>29</v>
@@ -9302,7 +9254,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="89" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B15" s="113" t="s">
         <v>30</v>
@@ -9336,7 +9288,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="89" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B16" s="113" t="s">
         <v>31</v>
@@ -9373,7 +9325,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="94" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C17" s="95">
         <v>0.45</v>
@@ -9406,7 +9358,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="89" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B19" s="113" t="s">
         <v>32</v>
@@ -9440,7 +9392,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="89" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B20" s="113" t="s">
         <v>33</v>
@@ -9492,7 +9444,7 @@
     </row>
     <row r="22" spans="1:10" s="14" customFormat="1">
       <c r="A22" s="89" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B22" s="113" t="s">
         <v>32</v>
@@ -9526,7 +9478,7 @@
     </row>
     <row r="23" spans="1:10" s="14" customFormat="1">
       <c r="A23" s="89" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B23" s="113" t="s">
         <v>33</v>
@@ -9596,7 +9548,7 @@
     </row>
     <row r="26" spans="1:10" s="14" customFormat="1">
       <c r="A26" s="89" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B26" s="113" t="s">
         <v>50</v>
@@ -9631,7 +9583,7 @@
     <row r="27" spans="1:10">
       <c r="A27" s="16"/>
       <c r="B27" s="13" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C27" s="119">
         <v>1</v>
@@ -9690,67 +9642,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
-      <c r="A1" s="216" t="s">
-        <v>309</v>
-      </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
+      <c r="A1" s="218" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
     </row>
     <row r="2" spans="1:10" ht="21">
-      <c r="A2" s="217" t="s">
-        <v>308</v>
-      </c>
-      <c r="B2" s="217"/>
-      <c r="C2" s="217"/>
-      <c r="D2" s="217"/>
-      <c r="E2" s="217"/>
-      <c r="F2" s="217"/>
-      <c r="G2" s="217"/>
-      <c r="H2" s="217"/>
-      <c r="I2" s="217"/>
-      <c r="J2" s="217"/>
+      <c r="A2" s="219" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="219"/>
+      <c r="C2" s="219"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="219"/>
+      <c r="F2" s="219"/>
+      <c r="G2" s="219"/>
+      <c r="H2" s="219"/>
+      <c r="I2" s="219"/>
+      <c r="J2" s="219"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="219" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="219"/>
-      <c r="C3" s="219"/>
-      <c r="D3" s="219"/>
-      <c r="E3" s="219"/>
-      <c r="F3" s="219"/>
-      <c r="G3" s="219"/>
-      <c r="H3" s="219"/>
-      <c r="I3" s="219"/>
-      <c r="J3" s="219"/>
+      <c r="A3" s="221" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="221"/>
+      <c r="C3" s="221"/>
+      <c r="D3" s="221"/>
+      <c r="E3" s="221"/>
+      <c r="F3" s="221"/>
+      <c r="G3" s="221"/>
+      <c r="H3" s="221"/>
+      <c r="I3" s="221"/>
+      <c r="J3" s="221"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="219" t="s">
-        <v>288</v>
-      </c>
-      <c r="B4" s="219"/>
-      <c r="C4" s="219"/>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
+      <c r="A4" s="221" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="221"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
+      <c r="H4" s="221"/>
+      <c r="I4" s="221"/>
+      <c r="J4" s="221"/>
     </row>
     <row r="6" spans="1:10" ht="47.25">
       <c r="A6" s="76" t="s">
         <v>279</v>
       </c>
       <c r="B6" s="76" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C6" s="76" t="s">
         <v>273</v>
@@ -9759,7 +9711,7 @@
         <v>177</v>
       </c>
       <c r="E6" s="76" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F6" s="77" t="s">
         <v>274</v>
@@ -9782,7 +9734,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="94" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C7" s="95">
         <v>0.2</v>
@@ -9800,7 +9752,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" s="97" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C8" s="98">
         <v>0.1</v>
@@ -9852,7 +9804,7 @@
         <v>1.2</v>
       </c>
       <c r="B10" s="100" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C10" s="101">
         <v>0.04</v>
@@ -9886,7 +9838,7 @@
         <v>1.3</v>
       </c>
       <c r="B11" s="100" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C11" s="101">
         <v>0.04</v>
@@ -9988,7 +9940,7 @@
         <v>1.2</v>
       </c>
       <c r="B14" s="106" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C14" s="107">
         <v>0.25</v>
@@ -10074,7 +10026,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="108" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C17" s="95">
         <v>0.45</v>
@@ -10294,7 +10246,7 @@
     <row r="24" spans="1:10" ht="21">
       <c r="A24" s="16"/>
       <c r="B24" s="110" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C24" s="112">
         <v>1</v>
@@ -10311,16 +10263,16 @@
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="G26" s="219" t="s">
-        <v>318</v>
-      </c>
-      <c r="H26" s="219"/>
-      <c r="I26" s="219"/>
-      <c r="J26" s="219"/>
+      <c r="G26" s="221" t="s">
+        <v>316</v>
+      </c>
+      <c r="H26" s="221"/>
+      <c r="I26" s="221"/>
+      <c r="J26" s="221"/>
     </row>
     <row r="27" spans="1:10">
       <c r="H27" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -10373,81 +10325,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
-      <c r="A1" s="216" t="s">
-        <v>309</v>
-      </c>
-      <c r="B1" s="216"/>
-      <c r="C1" s="216"/>
-      <c r="D1" s="216"/>
-      <c r="E1" s="216"/>
-      <c r="F1" s="216"/>
-      <c r="G1" s="216"/>
-      <c r="H1" s="216"/>
-      <c r="I1" s="216"/>
-      <c r="J1" s="216"/>
+      <c r="A1" s="218" t="s">
+        <v>307</v>
+      </c>
+      <c r="B1" s="218"/>
+      <c r="C1" s="218"/>
+      <c r="D1" s="218"/>
+      <c r="E1" s="218"/>
+      <c r="F1" s="218"/>
+      <c r="G1" s="218"/>
+      <c r="H1" s="218"/>
+      <c r="I1" s="218"/>
+      <c r="J1" s="218"/>
     </row>
     <row r="2" spans="1:10" ht="25.5">
-      <c r="A2" s="216" t="s">
+      <c r="A2" s="218" t="s">
         <v>179</v>
       </c>
-      <c r="B2" s="216"/>
-      <c r="C2" s="216"/>
-      <c r="D2" s="216"/>
-      <c r="E2" s="216"/>
-      <c r="F2" s="216"/>
-      <c r="G2" s="216"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="216"/>
-      <c r="J2" s="216"/>
+      <c r="B2" s="218"/>
+      <c r="C2" s="218"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="218"/>
+      <c r="F2" s="218"/>
+      <c r="G2" s="218"/>
+      <c r="H2" s="218"/>
+      <c r="I2" s="218"/>
+      <c r="J2" s="218"/>
     </row>
     <row r="3" spans="1:10" ht="18.75">
-      <c r="A3" s="218" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
-      <c r="H3" s="218"/>
-      <c r="I3" s="218"/>
-      <c r="J3" s="218"/>
+      <c r="A3" s="220" t="s">
+        <v>306</v>
+      </c>
+      <c r="B3" s="220"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
+      <c r="E3" s="220"/>
+      <c r="F3" s="220"/>
+      <c r="G3" s="220"/>
+      <c r="H3" s="220"/>
+      <c r="I3" s="220"/>
+      <c r="J3" s="220"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="219" t="s">
-        <v>287</v>
-      </c>
-      <c r="B4" s="219"/>
-      <c r="C4" s="219"/>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
+      <c r="A4" s="221" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" s="221"/>
+      <c r="C4" s="221"/>
+      <c r="D4" s="221"/>
+      <c r="E4" s="221"/>
+      <c r="F4" s="221"/>
+      <c r="G4" s="221"/>
+      <c r="H4" s="221"/>
+      <c r="I4" s="221"/>
+      <c r="J4" s="221"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="219" t="s">
-        <v>288</v>
-      </c>
-      <c r="B5" s="219"/>
-      <c r="C5" s="219"/>
-      <c r="D5" s="219"/>
-      <c r="E5" s="219"/>
-      <c r="F5" s="219"/>
-      <c r="G5" s="219"/>
-      <c r="H5" s="219"/>
-      <c r="I5" s="219"/>
-      <c r="J5" s="219"/>
+      <c r="A5" s="221" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" s="221"/>
+      <c r="C5" s="221"/>
+      <c r="D5" s="221"/>
+      <c r="E5" s="221"/>
+      <c r="F5" s="221"/>
+      <c r="G5" s="221"/>
+      <c r="H5" s="221"/>
+      <c r="I5" s="221"/>
+      <c r="J5" s="221"/>
     </row>
     <row r="7" spans="1:10" ht="47.25">
       <c r="A7" s="76" t="s">
         <v>279</v>
       </c>
       <c r="B7" s="76" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C7" s="76" t="s">
         <v>273</v>
@@ -10456,7 +10408,7 @@
         <v>177</v>
       </c>
       <c r="E7" s="76" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F7" s="77" t="s">
         <v>274</v>
@@ -10479,7 +10431,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="94" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C8" s="95">
         <v>0.2</v>
@@ -10497,7 +10449,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C9" s="98">
         <v>0.1</v>
@@ -10549,7 +10501,7 @@
         <v>1.2</v>
       </c>
       <c r="B11" s="100" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C11" s="101">
         <v>0.04</v>
@@ -10583,7 +10535,7 @@
         <v>1.3</v>
       </c>
       <c r="B12" s="100" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C12" s="101">
         <v>0.04</v>
@@ -10685,7 +10637,7 @@
         <v>1.2</v>
       </c>
       <c r="B15" s="106" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C15" s="107">
         <v>0.25</v>
@@ -10789,7 +10741,7 @@
         <v>2.1</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C19" s="3">
         <v>0.15</v>
@@ -10823,7 +10775,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C20" s="3">
         <v>0.1</v>
@@ -10855,7 +10807,7 @@
     <row r="21" spans="1:10" ht="21">
       <c r="A21" s="16"/>
       <c r="B21" s="110" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C21" s="112">
         <v>1</v>
@@ -10872,16 +10824,16 @@
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="E23" s="219" t="s">
-        <v>318</v>
-      </c>
-      <c r="F23" s="219"/>
-      <c r="G23" s="219"/>
-      <c r="H23" s="219"/>
+      <c r="E23" s="221" t="s">
+        <v>316</v>
+      </c>
+      <c r="F23" s="221"/>
+      <c r="G23" s="221"/>
+      <c r="H23" s="221"/>
     </row>
     <row r="24" spans="1:10">
       <c r="F24" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -11695,7 +11647,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
@@ -11734,7 +11686,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
@@ -11773,7 +11725,7 @@
         <v>1</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -11992,13 +11944,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12009,8 +11961,7 @@
     <col min="4" max="4" width="37.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.375" customWidth="1"/>
     <col min="6" max="6" width="21.375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="16.5" style="206" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="209" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
   </cols>
@@ -12034,10 +11985,10 @@
       <c r="F1" s="177" t="s">
         <v>118</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="216" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="216" t="s">
         <v>267</v>
       </c>
       <c r="I1" s="214" t="s">
@@ -12056,110 +12007,26 @@
         <v>1</v>
       </c>
       <c r="D2" s="57" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E2" s="57" t="s">
+        <v>336</v>
+      </c>
+      <c r="F2" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="F2" s="57" t="s">
-        <v>342</v>
-      </c>
-      <c r="G2" s="57">
+      <c r="G2" s="217">
         <v>1573185037185</v>
       </c>
-      <c r="H2" s="57"/>
+      <c r="H2" s="217"/>
       <c r="I2" s="208"/>
       <c r="J2" s="179">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="178">
-        <v>20</v>
-      </c>
-      <c r="B3" s="57">
-        <v>1</v>
-      </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57" t="s">
-        <v>339</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>339</v>
-      </c>
-      <c r="F3" s="57" t="s">
-        <v>343</v>
-      </c>
-      <c r="G3" s="57">
-        <v>1573185037185</v>
-      </c>
-      <c r="H3" s="57">
-        <v>1573185037184</v>
-      </c>
-      <c r="I3" s="208"/>
-      <c r="J3" s="179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="178">
-        <v>21</v>
-      </c>
-      <c r="B4" s="57">
-        <v>1</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57" t="s">
-        <v>340</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>340</v>
-      </c>
-      <c r="F4" s="57" t="s">
-        <v>344</v>
-      </c>
-      <c r="G4" s="57">
-        <v>1573185051583</v>
-      </c>
-      <c r="H4" s="57">
-        <v>1573185051583</v>
-      </c>
-      <c r="I4" s="208"/>
-      <c r="J4" s="179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="178">
-        <v>22</v>
-      </c>
-      <c r="B5" s="57">
-        <v>1</v>
-      </c>
-      <c r="C5" s="57"/>
-      <c r="D5" s="57" t="s">
-        <v>282</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>282</v>
-      </c>
-      <c r="F5" s="57" t="s">
-        <v>281</v>
-      </c>
-      <c r="G5" s="57">
-        <v>1573185071894</v>
-      </c>
-      <c r="H5" s="57">
-        <v>1573185071894</v>
-      </c>
-      <c r="I5" s="208"/>
-      <c r="J5" s="179">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -12173,10 +12040,10 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="9" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12244,7 +12111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="141.75">
+    <row r="2" spans="1:15" ht="19.5" customHeight="1">
       <c r="A2" s="92">
         <v>1</v>
       </c>
@@ -12258,10 +12125,10 @@
       <c r="G2" s="92"/>
       <c r="H2" s="92"/>
       <c r="I2" s="92" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="J2" s="92" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="K2" s="92"/>
       <c r="L2" s="207">
@@ -12271,13 +12138,13 @@
         <v>1573185131886</v>
       </c>
       <c r="N2" s="92" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="O2" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="141.75">
+    <row r="3" spans="1:15" ht="19.5" customHeight="1">
       <c r="A3" s="92">
         <v>2</v>
       </c>
@@ -12293,10 +12160,10 @@
       <c r="G3" s="92"/>
       <c r="H3" s="92"/>
       <c r="I3" s="92" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="J3" s="92" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="K3" s="92"/>
       <c r="L3" s="207">
@@ -12306,13 +12173,13 @@
         <v>1573185122446</v>
       </c>
       <c r="N3" s="92" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="O3" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="141.75">
+    <row r="4" spans="1:15" ht="23.25" customHeight="1">
       <c r="A4" s="92">
         <v>3</v>
       </c>
@@ -12328,10 +12195,10 @@
       <c r="G4" s="92"/>
       <c r="H4" s="92"/>
       <c r="I4" s="92" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="J4" s="92" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="K4" s="92"/>
       <c r="L4" s="207">
@@ -12341,13 +12208,13 @@
         <v>1573185164747</v>
       </c>
       <c r="N4" s="92" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="O4" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="141.75">
+    <row r="5" spans="1:15" ht="19.5" customHeight="1">
       <c r="A5" s="92">
         <v>4</v>
       </c>
@@ -12361,10 +12228,10 @@
       <c r="G5" s="92"/>
       <c r="H5" s="92"/>
       <c r="I5" s="92" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="J5" s="92" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="K5" s="92"/>
       <c r="L5" s="207">
@@ -12374,13 +12241,13 @@
         <v>1573185186458</v>
       </c>
       <c r="N5" s="92" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="O5" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="141.75">
+    <row r="6" spans="1:15" ht="20.25" customHeight="1">
       <c r="A6" s="92">
         <v>5</v>
       </c>
@@ -12396,10 +12263,10 @@
       <c r="G6" s="92"/>
       <c r="H6" s="92"/>
       <c r="I6" s="92" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="J6" s="92" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="K6" s="92"/>
       <c r="L6" s="207">
@@ -12409,13 +12276,13 @@
         <v>1573185204388</v>
       </c>
       <c r="N6" s="92" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="O6" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="141.75">
+    <row r="7" spans="1:15" ht="20.25" customHeight="1">
       <c r="A7" s="92">
         <v>6</v>
       </c>
@@ -12429,10 +12296,10 @@
       <c r="G7" s="92"/>
       <c r="H7" s="92"/>
       <c r="I7" s="92" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="J7" s="92" t="s">
-        <v>360</v>
+        <v>468</v>
       </c>
       <c r="K7" s="92"/>
       <c r="L7" s="207">
@@ -12442,7 +12309,7 @@
         <v>1573185232164</v>
       </c>
       <c r="N7" s="92" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="O7" s="92">
         <v>1</v>
@@ -12481,10 +12348,10 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1:O1048576"/>
+      <selection pane="bottomRight" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -12553,7 +12420,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="94.5">
+    <row r="2" spans="1:15" ht="22.5" customHeight="1">
       <c r="A2" s="92">
         <v>1</v>
       </c>
@@ -12563,7 +12430,7 @@
       <c r="C2" s="92"/>
       <c r="D2" s="92"/>
       <c r="E2" s="92" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="F2" s="92"/>
       <c r="G2" s="92"/>
@@ -12571,7 +12438,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="92" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="J2" s="92"/>
       <c r="K2" s="207">
@@ -12581,14 +12448,14 @@
         <v>1573185282750</v>
       </c>
       <c r="M2" s="92" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="N2" s="92"/>
       <c r="O2" s="92">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="94.5">
+    <row r="3" spans="1:15" ht="27" customHeight="1">
       <c r="A3" s="92">
         <v>2</v>
       </c>
@@ -12598,7 +12465,7 @@
       <c r="C3" s="92"/>
       <c r="D3" s="92"/>
       <c r="E3" s="92" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="F3" s="92"/>
       <c r="G3" s="92"/>
@@ -12606,7 +12473,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="92" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="J3" s="92"/>
       <c r="K3" s="207">
@@ -12616,7 +12483,7 @@
         <v>1573185368523</v>
       </c>
       <c r="M3" s="92" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="N3" s="92"/>
       <c r="O3" s="92">
@@ -12639,7 +12506,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -12662,49 +12529,49 @@
         <v>120</v>
       </c>
       <c r="C1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="D1" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="E1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F1" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="G1" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="H1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="I1" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="J1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="K1" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="L1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="M1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="N1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="O1" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="P1" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="Q1" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="R1" t="s">
         <v>15</v>
@@ -12719,10 +12586,10 @@
         <v>14</v>
       </c>
       <c r="V1" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="W1" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="X1" t="s">
         <v>9</v>
@@ -12730,28 +12597,28 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="D2">
         <v>766777123</v>
       </c>
       <c r="G2" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="H2" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="I2">
         <v>766777123</v>
       </c>
       <c r="J2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="M2">
         <v>99</v>
@@ -12760,7 +12627,7 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="P2" s="206">
         <v>1590118196428</v>
@@ -12769,7 +12636,7 @@
         <v>1591254395805</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="V2" s="206">
         <v>1573789598191</v>
@@ -12791,6 +12658,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x010100FB0175F18B01E74491971D89B23F8655" ma:contentTypeVersion="11" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="1a9dc9cdd67a308ba2b2666df5490aa6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="4c20e182-3cff-46d5-b163-30d344671daf" xmlns:ns4="c86ac200-3bf8-4f3f-9c75-7492a34ff116" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c3aad754d391d83d543dbc23cf02e780" ns3:_="" ns4:_="">
     <xsd:import namespace="4c20e182-3cff-46d5-b163-30d344671daf"/>
@@ -12999,15 +12875,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1F3B173-26E4-4636-A5EB-1C560CB0A9A3}">
   <ds:schemaRefs>
@@ -13026,6 +12893,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C10837DA-CF87-48E6-955F-4FAF14545FC0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F57D61BF-212A-4F3E-921D-E429A3A772FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -13042,12 +12917,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C10837DA-CF87-48E6-955F-4FAF14545FC0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>